<commit_message>
[expression] - [NUMBER]: **NEW** operation - `abs` - to convert a number into its absolute form (i.e. positive number).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/craigslist/artifact/data/SearchCraigslist.data.xlsx
+++ b/examples/craigslist/artifact/data/SearchCraigslist.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/examples/craigslist/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lium183/projects/nexial/tutorials/examples/craigslist/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518EF183-C849-D04B-887D-A8E0BF1C1C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431F87C0-BDA7-124D-8AB0-7CDAB5D42D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57600" yWindow="-14920" windowWidth="12800" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-28340" windowWidth="25600" windowHeight="28340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -1422,7 +1422,7 @@
         <v>134</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="7"/>

</xml_diff>